<commit_message>
divers ajustements SNT NSI et ESF
</commit_message>
<xml_diff>
--- a/content/docs/SNT_2nde/pages/pages_donnees/datas/fruits.xlsx
+++ b/content/docs/SNT_2nde/pages/pages_donnees/datas/fruits.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erictixidor/Documents/GitHub/hugo5/content/docs/SNT_2nde/pages/pages_donnees/datas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FCCA7B-8720-8C4F-94E3-1444CE47142E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C57ABFD-B974-E848-98E0-15097AE3D617}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14860" yWindow="500" windowWidth="13940" windowHeight="16440" xr2:uid="{804898C7-58A2-A748-988D-51F01FA4A5AB}"/>
   </bookViews>
@@ -153,7 +153,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFB6EE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -170,14 +170,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -192,6 +193,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFB6EE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -503,7 +509,7 @@
   <dimension ref="A2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,6 +525,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="1"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">

</xml_diff>